<commit_message>
dataset cleanup and common keywords
</commit_message>
<xml_diff>
--- a/DataSet/Party_DataSet/PTY_DataSet.xlsx
+++ b/DataSet/Party_DataSet/PTY_DataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Party_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E5CF7-1128-4ACC-A153-B2DFC6CEDA92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EB5A5A-FFB7-4126-85FA-66DF03E9758E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
   <si>
     <t>rowid</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>Australian Government, Fed Govt Dept or Auth</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>PTY005_PartyDetailsEnquiryReject</t>
   </si>
 </sst>
 </file>
@@ -770,7 +776,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP1" sqref="AP1"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1396,6 +1402,149 @@
         <v>106</v>
       </c>
     </row>
+    <row r="5" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>1414849</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" s="19">
+        <v>2020</v>
+      </c>
+      <c r="X5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>9890001</v>
+      </c>
+      <c r="AP5" s="2">
+        <v>67855555245</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
GDE-7217 - added test suite, data change, reordered resource file
</commit_message>
<xml_diff>
--- a/DataSet/Party_DataSet/PTY_DataSet.xlsx
+++ b/DataSet/Party_DataSet/PTY_DataSet.xlsx
@@ -438,11 +438,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CL39"/>
+  <dimension ref="A1:CL40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G19" sqref="G19"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="D12" s="26" t="inlineStr">
         <is>
-          <t>0711858</t>
+          <t>1615244</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
@@ -2700,12 +2700,12 @@
       </c>
       <c r="AN12" t="inlineStr">
         <is>
-          <t>Inner Works Inc 0711858</t>
+          <t>Inner Works Inc 1615244</t>
         </is>
       </c>
       <c r="AO12" t="inlineStr">
         <is>
-          <t>IW Inc_0711858</t>
+          <t>IW Inc_1615244</t>
         </is>
       </c>
     </row>
@@ -2906,20 +2906,22 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>PTY014_QuickEnterpriseParty_Validation_Mandatory_Fields</t>
+          <t>PTY012_DuplicateShortNameEdit_Party3</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Countryside Company</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>9890971</v>
+          <t>Sanseera Electronics Ltd</t>
+        </is>
+      </c>
+      <c r="D14" s="26" t="inlineStr">
+        <is>
+          <t>1710112</t>
+        </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>CS Comp</t>
+          <t>SE Ltd</t>
         </is>
       </c>
       <c r="F14" s="6" t="inlineStr">
@@ -2929,17 +2931,21 @@
       </c>
       <c r="G14" s="12" t="inlineStr">
         <is>
-          <t>00000001</t>
-        </is>
-      </c>
+          <t>00000852</t>
+        </is>
+      </c>
+      <c r="H14" s="12" t="n"/>
+      <c r="I14" s="6" t="n"/>
+      <c r="J14" s="6" t="n"/>
+      <c r="K14" s="6" t="n"/>
       <c r="L14" s="6" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="M14" s="2" t="inlineStr">
-        <is>
-          <t>Bank, Foreign Public Company Registered with ASIC</t>
+      <c r="M14" s="7" t="inlineStr">
+        <is>
+          <t>Formal Partnership, Joint Venture</t>
         </is>
       </c>
       <c r="N14" s="6" t="inlineStr">
@@ -2949,7 +2955,7 @@
       </c>
       <c r="O14" s="11" t="inlineStr">
         <is>
-          <t>0214201</t>
+          <t>1014001</t>
         </is>
       </c>
       <c r="P14" s="6" t="inlineStr">
@@ -2962,32 +2968,46 @@
           <t>2015-04-06</t>
         </is>
       </c>
-      <c r="R14" s="8" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="S14" s="8" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="T14" s="2" t="inlineStr">
-        <is>
-          <t>Finance and Insurance</t>
-        </is>
-      </c>
-      <c r="U14" s="2" t="inlineStr">
-        <is>
-          <t>Banks</t>
-        </is>
-      </c>
-      <c r="X14" s="11" t="inlineStr">
-        <is>
-          <t>30102020338</t>
-        </is>
-      </c>
-      <c r="Y14" s="6" t="n"/>
+      <c r="R14" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="S14" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="T14" s="6" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="U14" s="6" t="inlineStr">
+        <is>
+          <t>Higher Education</t>
+        </is>
+      </c>
+      <c r="V14" s="6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="W14" s="6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="X14" s="6" t="inlineStr">
+        <is>
+          <t>10075843210</t>
+        </is>
+      </c>
+      <c r="Y14" s="6" t="inlineStr">
+        <is>
+          <t>Legal Address</t>
+        </is>
+      </c>
       <c r="Z14" s="6" t="inlineStr">
         <is>
           <t>Australia</t>
@@ -2996,7 +3016,41 @@
       <c r="AA14" s="9" t="n">
         <v>2000</v>
       </c>
-      <c r="AH14" s="6" t="n"/>
+      <c r="AB14" s="6" t="inlineStr">
+        <is>
+          <t>LOWER GRND FL SHOP</t>
+        </is>
+      </c>
+      <c r="AC14" s="6" t="inlineStr">
+        <is>
+          <t>11 213 PITT ST</t>
+        </is>
+      </c>
+      <c r="AD14" s="2" t="inlineStr">
+        <is>
+          <t>Alnwick 3</t>
+        </is>
+      </c>
+      <c r="AE14" s="2" t="inlineStr">
+        <is>
+          <t>Northumberland 4</t>
+        </is>
+      </c>
+      <c r="AF14" s="10" t="inlineStr">
+        <is>
+          <t>Alnwick</t>
+        </is>
+      </c>
+      <c r="AG14" s="10" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="AH14" s="6" t="inlineStr">
+        <is>
+          <t>Documents not collected</t>
+        </is>
+      </c>
       <c r="AI14" s="6" t="inlineStr">
         <is>
           <t>Quick Party Onboarding</t>
@@ -3004,12 +3058,32 @@
       </c>
       <c r="AJ14" s="6" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="AK14" s="2" t="inlineStr">
         <is>
-          <t>Commonwealth Bank of Australia - DBU</t>
+          <t>CBA - Amsterdam</t>
+        </is>
+      </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>EU-EU</t>
+        </is>
+      </c>
+      <c r="AM14" t="inlineStr">
+        <is>
+          <t>Head Office</t>
+        </is>
+      </c>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>Sanseera Electronics Ltd 1710112</t>
+        </is>
+      </c>
+      <c r="AO14" t="inlineStr">
+        <is>
+          <t>SE Ltd_1710112</t>
         </is>
       </c>
     </row>
@@ -3021,17 +3095,20 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>PTY015_QuickPartyOnboarding_Validation_Disabled_Fields</t>
+          <t>PTY014_QuickEnterpriseParty_Validation_Mandatory_Fields</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>LINK Corp</t>
-        </is>
+          <t>Countryside Company</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>9890971</v>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>LK Crp</t>
+          <t>CS Comp</t>
         </is>
       </c>
       <c r="F15" s="6" t="inlineStr">
@@ -3044,10 +3121,6 @@
           <t>00000001</t>
         </is>
       </c>
-      <c r="H15" s="6" t="n"/>
-      <c r="I15" s="6" t="n"/>
-      <c r="J15" s="6" t="n"/>
-      <c r="K15" s="6" t="n"/>
       <c r="L15" s="6" t="inlineStr">
         <is>
           <t>Enterprise</t>
@@ -3055,7 +3128,7 @@
       </c>
       <c r="M15" s="2" t="inlineStr">
         <is>
-          <t>Superannuation Fund, Superannuation - Government Managed</t>
+          <t>Bank, Foreign Public Company Registered with ASIC</t>
         </is>
       </c>
       <c r="N15" s="6" t="inlineStr">
@@ -3063,11 +3136,56 @@
           <t>Full</t>
         </is>
       </c>
-      <c r="Z15" s="2" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
+      <c r="O15" s="11" t="inlineStr">
+        <is>
+          <t>0214201</t>
+        </is>
+      </c>
+      <c r="P15" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="Q15" s="8" t="inlineStr">
+        <is>
+          <t>2015-04-06</t>
+        </is>
+      </c>
+      <c r="R15" s="8" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="S15" s="8" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="T15" s="2" t="inlineStr">
+        <is>
+          <t>Finance and Insurance</t>
+        </is>
+      </c>
+      <c r="U15" s="2" t="inlineStr">
+        <is>
+          <t>Banks</t>
+        </is>
+      </c>
+      <c r="X15" s="11" t="inlineStr">
+        <is>
+          <t>30102020338</t>
+        </is>
+      </c>
+      <c r="Y15" s="6" t="n"/>
+      <c r="Z15" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="AA15" s="9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AH15" s="6" t="n"/>
       <c r="AI15" s="6" t="inlineStr">
         <is>
           <t>Quick Party Onboarding</t>
@@ -3083,7 +3201,6 @@
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="BB15" s="6" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="11" t="inlineStr">
@@ -3093,7 +3210,17 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>PTY016_PartyOnboarding_Validation_Branch</t>
+          <t>PTY015_QuickPartyOnboarding_Validation_Disabled_Fields</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>LINK Corp</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>LK Crp</t>
         </is>
       </c>
       <c r="F16" s="6" t="inlineStr">
@@ -3101,29 +3228,33 @@
           <t>Local Private</t>
         </is>
       </c>
-      <c r="G16" s="6" t="inlineStr">
-        <is>
-          <t>00000001|00000022</t>
-        </is>
-      </c>
-      <c r="H16" s="12" t="inlineStr">
+      <c r="G16" s="12" t="inlineStr">
         <is>
           <t>00000001</t>
         </is>
       </c>
-      <c r="I16" s="6" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia - DBU|Commonwealth Bank of Australia - OBU</t>
-        </is>
-      </c>
-      <c r="J16" s="6" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia|Commonwealth Bank of Australia</t>
-        </is>
-      </c>
-      <c r="K16" s="6" t="inlineStr">
-        <is>
-          <t>036|036</t>
+      <c r="H16" s="6" t="n"/>
+      <c r="I16" s="6" t="n"/>
+      <c r="J16" s="6" t="n"/>
+      <c r="K16" s="6" t="n"/>
+      <c r="L16" s="6" t="inlineStr">
+        <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="M16" s="2" t="inlineStr">
+        <is>
+          <t>Superannuation Fund, Superannuation - Government Managed</t>
+        </is>
+      </c>
+      <c r="N16" s="6" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="Z16" s="2" t="inlineStr">
+        <is>
+          <t>Australia</t>
         </is>
       </c>
       <c r="AI16" s="6" t="inlineStr">
@@ -3141,6 +3272,7 @@
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
+      <c r="BB16" s="6" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="11" t="inlineStr">
@@ -3150,36 +3282,92 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
+          <t>PTY016_PartyOnboarding_Validation_Branch</t>
+        </is>
+      </c>
+      <c r="F17" s="6" t="inlineStr">
+        <is>
+          <t>Local Private</t>
+        </is>
+      </c>
+      <c r="G17" s="6" t="inlineStr">
+        <is>
+          <t>00000001|00000022</t>
+        </is>
+      </c>
+      <c r="H17" s="12" t="inlineStr">
+        <is>
+          <t>00000001</t>
+        </is>
+      </c>
+      <c r="I17" s="6" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU|Commonwealth Bank of Australia - OBU</t>
+        </is>
+      </c>
+      <c r="J17" s="6" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia|Commonwealth Bank of Australia</t>
+        </is>
+      </c>
+      <c r="K17" s="6" t="inlineStr">
+        <is>
+          <t>036|036</t>
+        </is>
+      </c>
+      <c r="AI17" s="6" t="inlineStr">
+        <is>
+          <t>Quick Party Onboarding</t>
+        </is>
+      </c>
+      <c r="AJ17" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="AK17" s="2" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
           <t>PTY018_AU_Party_Navigation</t>
         </is>
       </c>
-      <c r="AJ17" s="6" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="AK17" s="2" t="inlineStr">
+      <c r="AJ18" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="AK18" s="2" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="AL17" t="inlineStr">
+      <c r="AL18" t="inlineStr">
         <is>
           <t>AU-AU</t>
         </is>
       </c>
-      <c r="BB17" s="6" t="inlineStr">
+      <c r="BB18" s="6" t="inlineStr">
         <is>
           <t>Europe</t>
         </is>
       </c>
-      <c r="BC17" s="2" t="inlineStr">
+      <c r="BC18" s="2" t="inlineStr">
         <is>
           <t>CBA - Amsterdam</t>
         </is>
       </c>
     </row>
-    <row r="18"/>
     <row r="19"/>
     <row r="20"/>
     <row r="21"/>
@@ -3197,29 +3385,30 @@
     <row r="33"/>
     <row r="34"/>
     <row r="35"/>
-    <row r="36">
-      <c r="C36" s="2" t="inlineStr">
+    <row r="36"/>
+    <row r="37">
+      <c r="C37" s="2" t="inlineStr">
         <is>
           <t>Columns available</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" s="5" t="inlineStr">
-        <is>
-          <t>Manual Input</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="13" t="inlineStr">
-        <is>
-          <t>Auto generated</t>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>Manual Input</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="15" t="inlineStr">
+      <c r="C39" s="13" t="inlineStr">
+        <is>
+          <t>Auto generated</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="15" t="inlineStr">
         <is>
           <t>New value</t>
         </is>

</xml_diff>

<commit_message>
GED-7217 - addressed review comments
</commit_message>
<xml_diff>
--- a/DataSet/Party_DataSet/PTY_DataSet.xlsx
+++ b/DataSet/Party_DataSet/PTY_DataSet.xlsx
@@ -438,11 +438,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CL40"/>
+  <dimension ref="A1:CL41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="D12" s="26" t="inlineStr">
         <is>
-          <t>1615244</t>
+          <t>1910852</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
@@ -2700,12 +2700,12 @@
       </c>
       <c r="AN12" t="inlineStr">
         <is>
-          <t>Inner Works Inc 1615244</t>
+          <t>Inner Works Inc 1910852</t>
         </is>
       </c>
       <c r="AO12" t="inlineStr">
         <is>
-          <t>IW Inc_1615244</t>
+          <t>IW Inc_1910852</t>
         </is>
       </c>
     </row>
@@ -2906,22 +2906,22 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>PTY012_DuplicateShortNameEdit_Party3</t>
+          <t>PTY012_DuplicateShortNameEdit_Party1</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd</t>
+          <t>Inner Works Inc</t>
         </is>
       </c>
       <c r="D14" s="26" t="inlineStr">
         <is>
-          <t>1710112</t>
+          <t>1912229</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>SE Ltd</t>
+          <t>IW Inc</t>
         </is>
       </c>
       <c r="F14" s="6" t="inlineStr">
@@ -2929,12 +2929,12 @@
           <t>Local Private</t>
         </is>
       </c>
-      <c r="G14" s="12" t="inlineStr">
-        <is>
-          <t>00000852</t>
-        </is>
-      </c>
-      <c r="H14" s="12" t="n"/>
+      <c r="G14" s="6" t="inlineStr">
+        <is>
+          <t>00000001</t>
+        </is>
+      </c>
+      <c r="H14" s="6" t="n"/>
       <c r="I14" s="6" t="n"/>
       <c r="J14" s="6" t="n"/>
       <c r="K14" s="6" t="n"/>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="M14" s="7" t="inlineStr">
         <is>
-          <t>Formal Partnership, Joint Venture</t>
+          <t>Unlisted Company, Foreign Public Company Registered with ASIC</t>
         </is>
       </c>
       <c r="N14" s="6" t="inlineStr">
@@ -2955,7 +2955,7 @@
       </c>
       <c r="O14" s="11" t="inlineStr">
         <is>
-          <t>1014001</t>
+          <t>9890002</t>
         </is>
       </c>
       <c r="P14" s="6" t="inlineStr">
@@ -2968,24 +2968,24 @@
           <t>2015-04-06</t>
         </is>
       </c>
-      <c r="R14" s="6" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="S14" s="6" t="inlineStr">
+      <c r="R14" s="8" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="S14" s="8" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
       <c r="T14" s="6" t="inlineStr">
         <is>
-          <t>Education</t>
+          <t>Electricity, Gas and Water Supply</t>
         </is>
       </c>
       <c r="U14" s="6" t="inlineStr">
         <is>
-          <t>Higher Education</t>
+          <t>Gas Supply</t>
         </is>
       </c>
       <c r="V14" s="6" t="inlineStr">
@@ -2998,9 +2998,9 @@
           <t>True</t>
         </is>
       </c>
-      <c r="X14" s="6" t="inlineStr">
-        <is>
-          <t>10075843210</t>
+      <c r="X14" s="12" t="inlineStr">
+        <is>
+          <t>67895843245</t>
         </is>
       </c>
       <c r="Y14" s="6" t="inlineStr">
@@ -3018,32 +3018,32 @@
       </c>
       <c r="AB14" s="6" t="inlineStr">
         <is>
-          <t>LOWER GRND FL SHOP</t>
+          <t xml:space="preserve">UPPER GRND FL </t>
         </is>
       </c>
       <c r="AC14" s="6" t="inlineStr">
         <is>
-          <t>11 213 PITT ST</t>
-        </is>
-      </c>
-      <c r="AD14" s="2" t="inlineStr">
-        <is>
-          <t>Alnwick 3</t>
-        </is>
-      </c>
-      <c r="AE14" s="2" t="inlineStr">
-        <is>
-          <t>Northumberland 4</t>
+          <t>10 SHIRLEY ST</t>
+        </is>
+      </c>
+      <c r="AD14" s="6" t="inlineStr">
+        <is>
+          <t>Pimpama Qld 3</t>
+        </is>
+      </c>
+      <c r="AE14" s="6" t="inlineStr">
+        <is>
+          <t>Pennyroyal 4</t>
         </is>
       </c>
       <c r="AF14" s="10" t="inlineStr">
         <is>
-          <t>Alnwick</t>
+          <t>Sydney</t>
         </is>
       </c>
       <c r="AG14" s="10" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>New South Wales</t>
         </is>
       </c>
       <c r="AH14" s="6" t="inlineStr">
@@ -3058,32 +3058,32 @@
       </c>
       <c r="AJ14" s="6" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="AK14" s="2" t="inlineStr">
         <is>
-          <t>CBA - Amsterdam</t>
+          <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>EU-EU</t>
+          <t>AU-AU</t>
         </is>
       </c>
       <c r="AM14" t="inlineStr">
         <is>
-          <t>Head Office</t>
+          <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
       <c r="AN14" t="inlineStr">
         <is>
-          <t>Sanseera Electronics Ltd 1710112</t>
+          <t>Inner Works Inc 1912229</t>
         </is>
       </c>
       <c r="AO14" t="inlineStr">
         <is>
-          <t>SE Ltd_1710112</t>
+          <t>IW Inc_1912229</t>
         </is>
       </c>
     </row>
@@ -3095,20 +3095,22 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>PTY014_QuickEnterpriseParty_Validation_Mandatory_Fields</t>
+          <t>PTY012_DuplicateShortNameEdit_Party2</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Countryside Company</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>9890971</v>
+          <t>Sanseera Electronics Ltd</t>
+        </is>
+      </c>
+      <c r="D15" s="26" t="inlineStr">
+        <is>
+          <t>1913100</t>
+        </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>CS Comp</t>
+          <t>SE Ltd</t>
         </is>
       </c>
       <c r="F15" s="6" t="inlineStr">
@@ -3118,17 +3120,21 @@
       </c>
       <c r="G15" s="12" t="inlineStr">
         <is>
-          <t>00000001</t>
-        </is>
-      </c>
+          <t>00000852</t>
+        </is>
+      </c>
+      <c r="H15" s="12" t="n"/>
+      <c r="I15" s="6" t="n"/>
+      <c r="J15" s="6" t="n"/>
+      <c r="K15" s="6" t="n"/>
       <c r="L15" s="6" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="M15" s="2" t="inlineStr">
-        <is>
-          <t>Bank, Foreign Public Company Registered with ASIC</t>
+      <c r="M15" s="7" t="inlineStr">
+        <is>
+          <t>Formal Partnership, Joint Venture</t>
         </is>
       </c>
       <c r="N15" s="6" t="inlineStr">
@@ -3138,7 +3144,7 @@
       </c>
       <c r="O15" s="11" t="inlineStr">
         <is>
-          <t>0214201</t>
+          <t>1014001</t>
         </is>
       </c>
       <c r="P15" s="6" t="inlineStr">
@@ -3151,32 +3157,46 @@
           <t>2015-04-06</t>
         </is>
       </c>
-      <c r="R15" s="8" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="S15" s="8" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="T15" s="2" t="inlineStr">
-        <is>
-          <t>Finance and Insurance</t>
-        </is>
-      </c>
-      <c r="U15" s="2" t="inlineStr">
-        <is>
-          <t>Banks</t>
-        </is>
-      </c>
-      <c r="X15" s="11" t="inlineStr">
-        <is>
-          <t>30102020338</t>
-        </is>
-      </c>
-      <c r="Y15" s="6" t="n"/>
+      <c r="R15" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="S15" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="T15" s="6" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="U15" s="6" t="inlineStr">
+        <is>
+          <t>Higher Education</t>
+        </is>
+      </c>
+      <c r="V15" s="6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="W15" s="6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="X15" s="6" t="inlineStr">
+        <is>
+          <t>10075843210</t>
+        </is>
+      </c>
+      <c r="Y15" s="6" t="inlineStr">
+        <is>
+          <t>Legal Address</t>
+        </is>
+      </c>
       <c r="Z15" s="6" t="inlineStr">
         <is>
           <t>Australia</t>
@@ -3185,7 +3205,41 @@
       <c r="AA15" s="9" t="n">
         <v>2000</v>
       </c>
-      <c r="AH15" s="6" t="n"/>
+      <c r="AB15" s="6" t="inlineStr">
+        <is>
+          <t>LOWER GRND FL SHOP</t>
+        </is>
+      </c>
+      <c r="AC15" s="6" t="inlineStr">
+        <is>
+          <t>11 213 PITT ST</t>
+        </is>
+      </c>
+      <c r="AD15" s="2" t="inlineStr">
+        <is>
+          <t>Alnwick 3</t>
+        </is>
+      </c>
+      <c r="AE15" s="2" t="inlineStr">
+        <is>
+          <t>Northumberland 4</t>
+        </is>
+      </c>
+      <c r="AF15" s="10" t="inlineStr">
+        <is>
+          <t>Alnwick</t>
+        </is>
+      </c>
+      <c r="AG15" s="10" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="AH15" s="6" t="inlineStr">
+        <is>
+          <t>Documents not collected</t>
+        </is>
+      </c>
       <c r="AI15" s="6" t="inlineStr">
         <is>
           <t>Quick Party Onboarding</t>
@@ -3193,12 +3247,32 @@
       </c>
       <c r="AJ15" s="6" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="AK15" s="2" t="inlineStr">
         <is>
-          <t>Commonwealth Bank of Australia - DBU</t>
+          <t>CBA - Amsterdam</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>EU-EU</t>
+        </is>
+      </c>
+      <c r="AM15" t="inlineStr">
+        <is>
+          <t>Head Office</t>
+        </is>
+      </c>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>Sanseera Electronics Ltd 1913100</t>
+        </is>
+      </c>
+      <c r="AO15" t="inlineStr">
+        <is>
+          <t>SE Ltd_1913100</t>
         </is>
       </c>
     </row>
@@ -3210,17 +3284,20 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>PTY015_QuickPartyOnboarding_Validation_Disabled_Fields</t>
+          <t>PTY014_QuickEnterpriseParty_Validation_Mandatory_Fields</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>LINK Corp</t>
-        </is>
+          <t>Countryside Company</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>9890971</v>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>LK Crp</t>
+          <t>CS Comp</t>
         </is>
       </c>
       <c r="F16" s="6" t="inlineStr">
@@ -3233,10 +3310,6 @@
           <t>00000001</t>
         </is>
       </c>
-      <c r="H16" s="6" t="n"/>
-      <c r="I16" s="6" t="n"/>
-      <c r="J16" s="6" t="n"/>
-      <c r="K16" s="6" t="n"/>
       <c r="L16" s="6" t="inlineStr">
         <is>
           <t>Enterprise</t>
@@ -3244,7 +3317,7 @@
       </c>
       <c r="M16" s="2" t="inlineStr">
         <is>
-          <t>Superannuation Fund, Superannuation - Government Managed</t>
+          <t>Bank, Foreign Public Company Registered with ASIC</t>
         </is>
       </c>
       <c r="N16" s="6" t="inlineStr">
@@ -3252,11 +3325,56 @@
           <t>Full</t>
         </is>
       </c>
-      <c r="Z16" s="2" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
+      <c r="O16" s="11" t="inlineStr">
+        <is>
+          <t>0214201</t>
+        </is>
+      </c>
+      <c r="P16" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="Q16" s="8" t="inlineStr">
+        <is>
+          <t>2015-04-06</t>
+        </is>
+      </c>
+      <c r="R16" s="8" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="S16" s="8" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="T16" s="2" t="inlineStr">
+        <is>
+          <t>Finance and Insurance</t>
+        </is>
+      </c>
+      <c r="U16" s="2" t="inlineStr">
+        <is>
+          <t>Banks</t>
+        </is>
+      </c>
+      <c r="X16" s="11" t="inlineStr">
+        <is>
+          <t>30102020338</t>
+        </is>
+      </c>
+      <c r="Y16" s="6" t="n"/>
+      <c r="Z16" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="AA16" s="9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="AH16" s="6" t="n"/>
       <c r="AI16" s="6" t="inlineStr">
         <is>
           <t>Quick Party Onboarding</t>
@@ -3272,7 +3390,6 @@
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="BB16" s="6" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="11" t="inlineStr">
@@ -3282,7 +3399,17 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>PTY016_PartyOnboarding_Validation_Branch</t>
+          <t>PTY015_QuickPartyOnboarding_Validation_Disabled_Fields</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>LINK Corp</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>LK Crp</t>
         </is>
       </c>
       <c r="F17" s="6" t="inlineStr">
@@ -3290,29 +3417,33 @@
           <t>Local Private</t>
         </is>
       </c>
-      <c r="G17" s="6" t="inlineStr">
-        <is>
-          <t>00000001|00000022</t>
-        </is>
-      </c>
-      <c r="H17" s="12" t="inlineStr">
+      <c r="G17" s="12" t="inlineStr">
         <is>
           <t>00000001</t>
         </is>
       </c>
-      <c r="I17" s="6" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia - DBU|Commonwealth Bank of Australia - OBU</t>
-        </is>
-      </c>
-      <c r="J17" s="6" t="inlineStr">
-        <is>
-          <t>Commonwealth Bank of Australia|Commonwealth Bank of Australia</t>
-        </is>
-      </c>
-      <c r="K17" s="6" t="inlineStr">
-        <is>
-          <t>036|036</t>
+      <c r="H17" s="6" t="n"/>
+      <c r="I17" s="6" t="n"/>
+      <c r="J17" s="6" t="n"/>
+      <c r="K17" s="6" t="n"/>
+      <c r="L17" s="6" t="inlineStr">
+        <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="M17" s="2" t="inlineStr">
+        <is>
+          <t>Superannuation Fund, Superannuation - Government Managed</t>
+        </is>
+      </c>
+      <c r="N17" s="6" t="inlineStr">
+        <is>
+          <t>Full</t>
+        </is>
+      </c>
+      <c r="Z17" s="2" t="inlineStr">
+        <is>
+          <t>Australia</t>
         </is>
       </c>
       <c r="AI17" s="6" t="inlineStr">
@@ -3330,6 +3461,7 @@
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
+      <c r="BB17" s="6" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="11" t="inlineStr">
@@ -3339,36 +3471,92 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
+          <t>PTY016_PartyOnboarding_Validation_Branch</t>
+        </is>
+      </c>
+      <c r="F18" s="6" t="inlineStr">
+        <is>
+          <t>Local Private</t>
+        </is>
+      </c>
+      <c r="G18" s="6" t="inlineStr">
+        <is>
+          <t>00000001|00000022</t>
+        </is>
+      </c>
+      <c r="H18" s="12" t="inlineStr">
+        <is>
+          <t>00000001</t>
+        </is>
+      </c>
+      <c r="I18" s="6" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU|Commonwealth Bank of Australia - OBU</t>
+        </is>
+      </c>
+      <c r="J18" s="6" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia|Commonwealth Bank of Australia</t>
+        </is>
+      </c>
+      <c r="K18" s="6" t="inlineStr">
+        <is>
+          <t>036|036</t>
+        </is>
+      </c>
+      <c r="AI18" s="6" t="inlineStr">
+        <is>
+          <t>Quick Party Onboarding</t>
+        </is>
+      </c>
+      <c r="AJ18" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="AK18" s="2" t="inlineStr">
+        <is>
+          <t>Commonwealth Bank of Australia - DBU</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
           <t>PTY018_AU_Party_Navigation</t>
         </is>
       </c>
-      <c r="AJ18" s="6" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="AK18" s="2" t="inlineStr">
+      <c r="AJ19" s="6" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="AK19" s="2" t="inlineStr">
         <is>
           <t>Commonwealth Bank of Australia - DBU</t>
         </is>
       </c>
-      <c r="AL18" t="inlineStr">
+      <c r="AL19" t="inlineStr">
         <is>
           <t>AU-AU</t>
         </is>
       </c>
-      <c r="BB18" s="6" t="inlineStr">
+      <c r="BB19" s="6" t="inlineStr">
         <is>
           <t>Europe</t>
         </is>
       </c>
-      <c r="BC18" s="2" t="inlineStr">
+      <c r="BC19" s="2" t="inlineStr">
         <is>
           <t>CBA - Amsterdam</t>
         </is>
       </c>
     </row>
-    <row r="19"/>
     <row r="20"/>
     <row r="21"/>
     <row r="22"/>
@@ -3386,29 +3574,30 @@
     <row r="34"/>
     <row r="35"/>
     <row r="36"/>
-    <row r="37">
-      <c r="C37" s="2" t="inlineStr">
+    <row r="37"/>
+    <row r="38">
+      <c r="C38" s="2" t="inlineStr">
         <is>
           <t>Columns available</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="C38" s="5" t="inlineStr">
-        <is>
-          <t>Manual Input</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="13" t="inlineStr">
-        <is>
-          <t>Auto generated</t>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>Manual Input</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="C40" s="15" t="inlineStr">
+      <c r="C40" s="13" t="inlineStr">
+        <is>
+          <t>Auto generated</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" s="15" t="inlineStr">
         <is>
           <t>New value</t>
         </is>

</xml_diff>

<commit_message>
GDE-7247 - addressed review comments
</commit_message>
<xml_diff>
--- a/DataSet/Party_DataSet/PTY_DataSet.xlsx
+++ b/DataSet/Party_DataSet/PTY_DataSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u711091\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_Evergreen\fms_cba\DataSet\Party_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E9EB3-995A-4B5F-B66E-7397AD713496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E772B192-D48A-416C-BD4C-9C7D2E706E3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7770" windowWidth="28800" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="286">
   <si>
     <t>rowid</t>
   </si>
@@ -742,28 +742,142 @@
     <t>20</t>
   </si>
   <si>
+    <t>Number_of_Parties</t>
+  </si>
+  <si>
+    <t>Default_Address</t>
+  </si>
+  <si>
+    <t>Is_Internet</t>
+  </si>
+  <si>
+    <t>Is_Mobile</t>
+  </si>
+  <si>
+    <t>Is_Tax_Payer</t>
+  </si>
+  <si>
+    <t>Non_Resident_License_Permit</t>
+  </si>
+  <si>
+    <t>Franchise_Affinity</t>
+  </si>
+  <si>
+    <t>Import_Export</t>
+  </si>
+  <si>
+    <t>PTY006_BulkPartyUpload</t>
+  </si>
+  <si>
+    <t>AGS</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>AFFINITY</t>
+  </si>
+  <si>
+    <t>BOTH</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>AUS_810P</t>
+  </si>
+  <si>
+    <t>AUS_8112</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>LINE 1</t>
+  </si>
+  <si>
+    <t>LINE 2</t>
+  </si>
+  <si>
+    <t>LINE 3</t>
+  </si>
+  <si>
+    <t>LINE 4</t>
+  </si>
+  <si>
+    <t>SYDNEY</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Bulk Party Upload</t>
+  </si>
+  <si>
+    <t>COMRLENDING</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Save_Path</t>
+  </si>
+  <si>
+    <t>C:\GIT_Evergreen\fms_cba\DataSet\Party_DataSet\</t>
+  </si>
+  <si>
+    <t>Valid_GLApplication</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>PTY020_PartyCrossReferenceDetails</t>
+  </si>
+  <si>
+    <t>Kiddeo Corp</t>
+  </si>
+  <si>
+    <t>1512635</t>
+  </si>
+  <si>
+    <t>KD Crp</t>
+  </si>
+  <si>
+    <t>Accommodation</t>
+  </si>
+  <si>
     <t>COMRLENDING|PARTY</t>
   </si>
   <si>
-    <t>Accommodation</t>
-  </si>
-  <si>
-    <t>KD Crp</t>
-  </si>
-  <si>
-    <t>1512635</t>
-  </si>
-  <si>
-    <t>Kiddeo Corp</t>
-  </si>
-  <si>
-    <t>PTY020_PartyCrossReferenceDetails</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Valid_GLApplication</t>
+    <t>Party_Type_Code</t>
+  </si>
+  <si>
+    <t>Party_Sub_Type_Code</t>
+  </si>
+  <si>
+    <t>State_Province_Code</t>
+  </si>
+  <si>
+    <t>Address_Type_Code</t>
+  </si>
+  <si>
+    <t>Industry_Sector_Code</t>
+  </si>
+  <si>
+    <t>Business_Activity_Code</t>
+  </si>
+  <si>
+    <t>Australian Government, State Govt Dept or Auth</t>
+  </si>
+  <si>
+    <t>Government Administration</t>
+  </si>
+  <si>
+    <t>State Government Administration</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1320,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CL43"/>
+  <dimension ref="A1:CU44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B28" sqref="B28"/>
+      <pane xSplit="2" topLeftCell="BM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BN6" sqref="BN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1225,69 +1339,69 @@
     <col min="12" max="12" width="11.140625" style="2" customWidth="1"/>
     <col min="13" max="13" width="46.5703125" style="2" customWidth="1"/>
     <col min="14" max="14" width="15" style="2" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="24.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="23" style="2" customWidth="1"/>
-    <col min="20" max="20" width="27.28515625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="28.5703125" style="2" customWidth="1"/>
-    <col min="22" max="24" width="15.5703125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="10.5703125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="35.42578125" style="2" customWidth="1"/>
-    <col min="29" max="31" width="15.28515625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" style="2" customWidth="1"/>
-    <col min="33" max="33" width="14.85546875" style="2" customWidth="1"/>
-    <col min="34" max="34" width="38.28515625" style="2" customWidth="1"/>
-    <col min="35" max="35" width="21.140625" style="2" customWidth="1"/>
-    <col min="36" max="36" width="28.85546875" style="2" customWidth="1"/>
-    <col min="37" max="37" width="37.42578125" style="2" customWidth="1"/>
-    <col min="38" max="38" width="23" style="2" customWidth="1"/>
-    <col min="39" max="39" width="19.85546875" style="2" customWidth="1"/>
-    <col min="40" max="40" width="23.28515625" style="2" customWidth="1"/>
-    <col min="41" max="42" width="19.85546875" style="2" customWidth="1"/>
-    <col min="43" max="44" width="24.7109375" style="2" customWidth="1"/>
-    <col min="45" max="45" width="25" style="2" customWidth="1"/>
-    <col min="46" max="46" width="24.42578125" style="2" customWidth="1"/>
-    <col min="47" max="47" width="30.42578125" style="2" customWidth="1"/>
-    <col min="48" max="48" width="36" style="2" customWidth="1"/>
-    <col min="49" max="49" width="34.42578125" style="2" customWidth="1"/>
-    <col min="50" max="50" width="26.7109375" style="2" customWidth="1"/>
-    <col min="51" max="52" width="17.28515625" style="2" customWidth="1"/>
-    <col min="53" max="53" width="34.140625" style="2" customWidth="1"/>
-    <col min="54" max="54" width="28.42578125" style="2" customWidth="1"/>
-    <col min="55" max="55" width="24.7109375" style="2" customWidth="1"/>
-    <col min="56" max="56" width="28.42578125" style="2" customWidth="1"/>
-    <col min="57" max="57" width="24.7109375" style="2" customWidth="1"/>
-    <col min="58" max="58" width="30.28515625" style="2" customWidth="1"/>
-    <col min="59" max="59" width="17.5703125" style="2" customWidth="1"/>
-    <col min="60" max="60" width="20.28515625" style="2" customWidth="1"/>
-    <col min="61" max="61" width="12.140625" style="2" customWidth="1"/>
-    <col min="62" max="62" width="21.42578125" style="2" customWidth="1"/>
-    <col min="63" max="63" width="24.140625" style="2" customWidth="1"/>
-    <col min="64" max="64" width="16" style="2" customWidth="1"/>
-    <col min="65" max="65" width="14" style="2" customWidth="1"/>
-    <col min="66" max="66" width="16.7109375" style="2" customWidth="1"/>
-    <col min="67" max="67" width="10.42578125" style="2" customWidth="1"/>
-    <col min="68" max="68" width="37.7109375" style="2" customWidth="1"/>
-    <col min="69" max="70" width="16.7109375" style="2" customWidth="1"/>
-    <col min="71" max="73" width="20.140625" style="2" customWidth="1"/>
-    <col min="74" max="74" width="17.7109375" style="2" customWidth="1"/>
-    <col min="75" max="75" width="24.5703125" style="2" customWidth="1"/>
-    <col min="76" max="78" width="19.42578125" style="2" customWidth="1"/>
-    <col min="79" max="79" width="21.140625" style="2" customWidth="1"/>
-    <col min="80" max="80" width="32.42578125" style="2" customWidth="1"/>
-    <col min="81" max="82" width="17.28515625" style="2" customWidth="1"/>
-    <col min="83" max="85" width="17.5703125" style="2" customWidth="1"/>
-    <col min="86" max="86" width="26.28515625" style="2" customWidth="1"/>
-    <col min="87" max="87" width="35" style="2" customWidth="1"/>
-    <col min="88" max="88" width="26.5703125" style="2" customWidth="1"/>
-    <col min="89" max="89" width="24.85546875" style="2" customWidth="1"/>
-    <col min="90" max="90" width="20" style="2" customWidth="1"/>
+    <col min="15" max="21" width="19.140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" style="2" customWidth="1"/>
+    <col min="24" max="25" width="23" style="2" customWidth="1"/>
+    <col min="26" max="26" width="27.28515625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="28.5703125" style="2" customWidth="1"/>
+    <col min="28" max="30" width="15.5703125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" style="2" customWidth="1"/>
+    <col min="32" max="32" width="15.5703125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="10.5703125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="35.42578125" style="2" customWidth="1"/>
+    <col min="35" max="37" width="15.28515625" style="2" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" style="2" customWidth="1"/>
+    <col min="39" max="40" width="14.85546875" style="2" customWidth="1"/>
+    <col min="41" max="41" width="38.28515625" style="2" customWidth="1"/>
+    <col min="42" max="42" width="21.140625" style="2" customWidth="1"/>
+    <col min="43" max="43" width="28.85546875" style="2" customWidth="1"/>
+    <col min="44" max="44" width="37.42578125" style="2" customWidth="1"/>
+    <col min="45" max="45" width="23" style="2" customWidth="1"/>
+    <col min="46" max="46" width="19.85546875" style="2" customWidth="1"/>
+    <col min="47" max="47" width="23.28515625" style="2" customWidth="1"/>
+    <col min="48" max="49" width="19.85546875" style="2" customWidth="1"/>
+    <col min="50" max="51" width="24.7109375" style="2" customWidth="1"/>
+    <col min="52" max="52" width="25" style="2" customWidth="1"/>
+    <col min="53" max="53" width="24.42578125" style="2" customWidth="1"/>
+    <col min="54" max="54" width="30.42578125" style="2" customWidth="1"/>
+    <col min="55" max="55" width="36" style="2" customWidth="1"/>
+    <col min="56" max="56" width="34.42578125" style="2" customWidth="1"/>
+    <col min="57" max="57" width="26.7109375" style="2" customWidth="1"/>
+    <col min="58" max="59" width="17.28515625" style="2" customWidth="1"/>
+    <col min="60" max="60" width="34.140625" style="2" customWidth="1"/>
+    <col min="61" max="61" width="28.42578125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="24.7109375" style="2" customWidth="1"/>
+    <col min="63" max="63" width="28.42578125" style="2" customWidth="1"/>
+    <col min="64" max="64" width="24.7109375" style="2" customWidth="1"/>
+    <col min="65" max="67" width="30.28515625" style="2" customWidth="1"/>
+    <col min="68" max="68" width="21.140625" style="2" customWidth="1"/>
+    <col min="69" max="69" width="20.28515625" style="2" customWidth="1"/>
+    <col min="70" max="70" width="22" style="2" customWidth="1"/>
+    <col min="71" max="71" width="21.42578125" style="2" customWidth="1"/>
+    <col min="72" max="72" width="24.140625" style="2" customWidth="1"/>
+    <col min="73" max="73" width="21.5703125" style="2" customWidth="1"/>
+    <col min="74" max="74" width="23.140625" style="2" customWidth="1"/>
+    <col min="75" max="75" width="16.7109375" style="2" customWidth="1"/>
+    <col min="76" max="76" width="10.42578125" style="2" customWidth="1"/>
+    <col min="77" max="77" width="37.7109375" style="2" customWidth="1"/>
+    <col min="78" max="79" width="16.7109375" style="2" customWidth="1"/>
+    <col min="80" max="82" width="20.140625" style="2" customWidth="1"/>
+    <col min="83" max="83" width="17.7109375" style="2" customWidth="1"/>
+    <col min="84" max="84" width="24.5703125" style="2" customWidth="1"/>
+    <col min="85" max="87" width="19.42578125" style="2" customWidth="1"/>
+    <col min="88" max="88" width="21.140625" style="2" customWidth="1"/>
+    <col min="89" max="89" width="32.42578125" style="2" customWidth="1"/>
+    <col min="90" max="91" width="17.28515625" style="2" customWidth="1"/>
+    <col min="92" max="94" width="17.5703125" style="2" customWidth="1"/>
+    <col min="95" max="95" width="26.28515625" style="2" customWidth="1"/>
+    <col min="96" max="96" width="35" style="2" customWidth="1"/>
+    <col min="97" max="97" width="26.5703125" style="2" customWidth="1"/>
+    <col min="98" max="98" width="24.85546875" style="2" customWidth="1"/>
+    <col min="99" max="99" width="20" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1334,152 +1448,182 @@
         <v>14</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="AO1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AT1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AU1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AV1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="BC1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="BD1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="BE1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="BF1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BH1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BI1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BK1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BL1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BM1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="BH1" s="5"/>
-      <c r="BI1" s="5"/>
-      <c r="BJ1" s="5"/>
-      <c r="BK1" s="5"/>
-      <c r="BL1" s="5"/>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
-      <c r="BO1" s="5"/>
-      <c r="BP1" s="5"/>
-      <c r="BQ1" s="5"/>
-      <c r="BR1" s="5"/>
-      <c r="BS1" s="5"/>
-      <c r="BT1" s="5"/>
-      <c r="BU1" s="5"/>
-      <c r="BV1" s="5"/>
+      <c r="BN1" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="BT1" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>282</v>
+      </c>
       <c r="BW1" s="5"/>
       <c r="BX1" s="5"/>
       <c r="BY1" s="5"/>
@@ -1496,8 +1640,17 @@
       <c r="CJ1" s="5"/>
       <c r="CK1" s="5"/>
       <c r="CL1" s="5"/>
+      <c r="CM1" s="5"/>
+      <c r="CN1" s="5"/>
+      <c r="CO1" s="5"/>
+      <c r="CP1" s="5"/>
+      <c r="CQ1" s="5"/>
+      <c r="CR1" s="5"/>
+      <c r="CS1" s="5"/>
+      <c r="CT1" s="5"/>
+      <c r="CU1" s="5"/>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>57</v>
       </c>
@@ -1535,77 +1688,84 @@
       <c r="O2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T2" s="6" t="s">
+      <c r="X2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="AD2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA2" s="9">
+      <c r="AF2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG2" s="9">
         <v>2000</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AF2" s="10" t="s">
+      <c r="AL2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AM2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AQ2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
     </row>
-    <row r="3" spans="1:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>84</v>
       </c>
@@ -1643,77 +1803,84 @@
       <c r="O3" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" s="18" t="s">
+      <c r="X3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z3" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="AA3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="AD3" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA3" s="19">
+      <c r="AF3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG3" s="19">
         <v>2020</v>
       </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AH3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="AC3" s="14" t="s">
+      <c r="AI3" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AD3" s="18" t="s">
+      <c r="AJ3" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="AE3" s="18" t="s">
+      <c r="AK3" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AL3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AG3" s="14" t="s">
+      <c r="AM3" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AJ3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AQ3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
     </row>
-    <row r="4" spans="1:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>100</v>
       </c>
@@ -1751,107 +1918,114 @@
       <c r="O4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" s="8" t="s">
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T4" s="6" t="s">
+      <c r="X4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="AB4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="AC4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X4" s="17" t="s">
+      <c r="AD4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="AE4" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA4" s="19">
+      <c r="AF4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" s="19">
         <v>2020</v>
       </c>
-      <c r="AB4" s="18" t="s">
+      <c r="AH4" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="AC4" s="14" t="s">
+      <c r="AI4" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="AD4" s="18" t="s">
+      <c r="AJ4" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="AE4" s="18" t="s">
+      <c r="AK4" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="AF4" s="14" t="s">
+      <c r="AL4" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="AG4" s="14" t="s">
+      <c r="AM4" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="AH4" s="6" t="s">
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI4" s="2" t="s">
+      <c r="AP4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AJ4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK4" s="2" t="s">
+      <c r="AQ4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL4"/>
-      <c r="AM4"/>
-      <c r="AN4"/>
-      <c r="AQ4" s="2" t="s">
+      <c r="AS4"/>
+      <c r="AT4"/>
+      <c r="AU4"/>
+      <c r="AX4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AZ4" s="2">
         <v>9890001</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="BA4" s="2">
         <v>67855555245</v>
       </c>
-      <c r="AU4" s="2" t="s">
+      <c r="BB4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AV4" s="2">
+      <c r="BC4" s="2">
         <v>1</v>
       </c>
-      <c r="AW4" s="2">
+      <c r="BD4" s="2">
         <v>0</v>
       </c>
-      <c r="AX4" s="2">
+      <c r="BE4" s="2">
         <v>0</v>
       </c>
-      <c r="AY4" s="2" t="s">
+      <c r="BF4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AZ4" s="2">
+      <c r="BG4" s="2">
         <v>0</v>
       </c>
-      <c r="BA4" s="2" t="s">
+      <c r="BH4" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>110</v>
       </c>
@@ -1889,218 +2063,290 @@
       <c r="O5" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" s="8" t="s">
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" s="6" t="s">
+      <c r="X5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="AA5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="AB5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="AC5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X5" s="22" t="s">
+      <c r="AD5" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="AE5" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Z5" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA5" s="24">
+      <c r="AF5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG5" s="24">
         <v>2020</v>
       </c>
-      <c r="AB5" s="23" t="s">
+      <c r="AH5" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AC5" s="20" t="s">
+      <c r="AI5" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="AD5" s="23" t="s">
+      <c r="AJ5" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="AE5" s="23" t="s">
+      <c r="AK5" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="AF5" s="20" t="s">
+      <c r="AL5" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="AG5" s="20" t="s">
+      <c r="AM5" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="AH5" s="23" t="s">
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="AI5" s="23" t="s">
+      <c r="AP5" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="AJ5" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK5" s="2" t="s">
+      <c r="AQ5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL5"/>
-      <c r="AM5"/>
-      <c r="AN5"/>
-      <c r="AQ5" s="2" t="s">
+      <c r="AS5"/>
+      <c r="AT5"/>
+      <c r="AU5"/>
+      <c r="AX5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AZ5" s="2">
         <v>9890001</v>
       </c>
-      <c r="AT5" s="2">
+      <c r="BA5" s="2">
         <v>67855555245</v>
       </c>
-      <c r="AU5" s="2" t="s">
+      <c r="BB5" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AV5" s="2">
+      <c r="BC5" s="2">
         <v>1</v>
       </c>
-      <c r="AW5" s="2">
+      <c r="BD5" s="2">
         <v>0</v>
       </c>
-      <c r="AX5" s="2">
+      <c r="BE5" s="2">
         <v>0</v>
       </c>
-      <c r="AY5" s="2" t="s">
+      <c r="BF5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AZ5" s="2">
+      <c r="BG5" s="2">
         <v>0</v>
       </c>
-      <c r="BA5" s="2" t="s">
+      <c r="BH5" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>248</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D6" s="26"/>
       <c r="E6" s="2" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="26" t="s">
         <v>63</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" t="s">
+        <v>253</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>118</v>
+      <c r="M6" t="s">
+        <v>283</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>120</v>
+        <v>250</v>
+      </c>
+      <c r="O6"/>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6"/>
+      <c r="T6" t="s">
+        <v>251</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="X6" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y6" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>284</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>285</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>12312312312</v>
+      </c>
+      <c r="AE6" t="s">
         <v>74</v>
       </c>
-      <c r="Z6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA6" s="24">
+      <c r="AF6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG6">
         <v>2000</v>
       </c>
-      <c r="AB6" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF6" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG6" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH6" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AH6" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>259</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>260</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>263</v>
+      </c>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AM6"/>
-      <c r="AN6"/>
+      <c r="AS6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU6"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="BA6" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>265</v>
+      </c>
+      <c r="BF6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="2">
+        <v>5</v>
+      </c>
+      <c r="BO6" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="BQ6" s="2">
+        <v>1063</v>
+      </c>
+      <c r="BR6" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BS6" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BT6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="BU6" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="BV6" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="CT6"/>
+      <c r="CU6"/>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>127</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>116</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>62</v>
@@ -2108,43 +2354,103 @@
       <c r="G7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AI7" s="6" t="s">
+      <c r="O7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE7" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG7" s="24">
+        <v>2000</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL7" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM7" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK7" s="2" t="s">
+      <c r="AQ7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AM7"/>
-      <c r="AN7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>131</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>62</v>
@@ -2152,264 +2458,224 @@
       <c r="G8" s="12" t="s">
         <v>63</v>
       </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="X8" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y8" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA8" s="24">
-        <v>2000</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF8" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG8" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AI8" s="6" t="s">
+      <c r="AP8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK8" s="2" t="s">
+      <c r="AQ8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AM8"/>
-      <c r="AN8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+        <v>63</v>
+      </c>
       <c r="L9" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="8"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="24"/>
-      <c r="AI9" s="6" t="s">
+      <c r="O9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE9" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG9" s="24">
+        <v>2000</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM9" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN9" s="20"/>
+      <c r="AO9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ9" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AK9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AN9" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="BD9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="BE9" s="2" t="s">
+      <c r="AQ9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BF9" s="2" t="s">
-        <v>151</v>
-      </c>
+      <c r="AT9"/>
+      <c r="AU9"/>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>152</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>63</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O10" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="V10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="X10" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y10" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA10" s="24">
-        <v>2000</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF10" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG10" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH10" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AI10" s="6" t="s">
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="8"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="24"/>
+      <c r="AP10" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK10" s="2" t="s">
+      <c r="AQ10" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU10" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="BK10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="BL10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AM10"/>
-      <c r="AN10"/>
+      <c r="BM10" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>165</v>
+        <v>154</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>62</v>
@@ -2417,288 +2683,309 @@
       <c r="G11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
       <c r="L11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>66</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q11" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T11" s="2" t="s">
+      <c r="X11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="AA11" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="V11" s="6" t="s">
+      <c r="AB11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W11" s="6" t="s">
+      <c r="AC11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X11" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="Y11" s="23" t="s">
+      <c r="AD11" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE11" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Z11" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA11" s="24">
-        <v>2020</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AC11" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AF11" s="2" t="s">
-        <v>171</v>
+      <c r="AF11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG11" s="24">
+        <v>2000</v>
       </c>
       <c r="AH11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL11" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM11" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN11" s="20"/>
+      <c r="AO11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI11" s="6" t="s">
+      <c r="AP11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK11" s="2" t="s">
+      <c r="AQ11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR11" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="AT11"/>
+      <c r="AU11"/>
     </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>172</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>146</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>66</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q12" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W12" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R12" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="V12" s="6" t="s">
+      <c r="X12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W12" s="6" t="s">
+      <c r="AC12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X12" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y12" s="23" t="s">
+      <c r="AD12" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE12" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Z12" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA12" s="24">
-        <v>1011</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AE12" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="AF12" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="AG12" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="AH12" s="6" t="s">
+      <c r="AF12" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG12" s="24">
+        <v>2020</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL12" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AI12" s="6" t="s">
+      <c r="AP12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ12" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AK12" s="2" t="s">
-        <v>149</v>
+      <c r="AQ12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR12" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>179</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+        <v>146</v>
+      </c>
       <c r="L13" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>66</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="W13" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="V13" s="6" t="s">
+      <c r="X13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W13" s="6" t="s">
+      <c r="AC13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X13" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y13" s="23" t="s">
+      <c r="AD13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE13" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Z13" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA13" s="24">
-        <v>2020</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AF13" s="2" t="s">
-        <v>171</v>
+      <c r="AF13" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG13" s="24">
+        <v>1011</v>
       </c>
       <c r="AH13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK13" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL13" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM13" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN13" s="10"/>
+      <c r="AO13" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI13" s="6" t="s">
+      <c r="AP13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK13" s="2" t="s">
-        <v>83</v>
+      <c r="AQ13" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>185</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="12" t="s">
         <v>63</v>
       </c>
       <c r="H14" s="6"/>
@@ -2708,109 +2995,94 @@
       <c r="L14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>65</v>
+      <c r="M14" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="N14" s="6" t="s">
         <v>66</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q14" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W14" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R14" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="V14" s="6" t="s">
+      <c r="X14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W14" s="6" t="s">
+      <c r="AC14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X14" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y14" s="6" t="s">
+      <c r="AD14" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE14" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="Z14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA14" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AB14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD14" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG14" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH14" s="6" t="s">
+      <c r="AF14" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG14" s="24">
+        <v>2020</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AI14" s="6" t="s">
+      <c r="AP14" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK14" s="2" t="s">
+      <c r="AQ14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>211</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>212</v>
-      </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>192</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>86</v>
+        <v>209</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>87</v>
+        <v>210</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>62</v>
@@ -2825,109 +3097,116 @@
       <c r="L15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M15" s="16" t="s">
-        <v>88</v>
+      <c r="M15" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O15" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q15" s="8" t="s">
+      <c r="O15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T15" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="U15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="V15" s="6" t="s">
+      <c r="X15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W15" s="6" t="s">
+      <c r="AC15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X15" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y15" s="6" t="s">
+      <c r="AD15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE15" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA15" s="19">
-        <v>2020</v>
-      </c>
-      <c r="AB15" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC15" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD15" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE15" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF15" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG15" s="14" t="s">
-        <v>98</v>
+      <c r="AF15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>2000</v>
       </c>
       <c r="AH15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN15" s="10"/>
+      <c r="AO15" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI15" s="6" t="s">
+      <c r="AP15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK15" s="2" t="s">
+      <c r="AQ15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AS15" t="s">
         <v>106</v>
       </c>
-      <c r="AM15" t="s">
+      <c r="AT15" t="s">
         <v>83</v>
       </c>
-      <c r="AN15" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="AO15" s="2" t="s">
-        <v>216</v>
+      <c r="AU15" t="s">
+        <v>211</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>213</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>61</v>
+        <v>214</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>62</v>
@@ -2942,117 +3221,124 @@
       <c r="L16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M16" s="7" t="s">
-        <v>65</v>
+      <c r="M16" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q16" s="8" t="s">
+      <c r="O16" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S16" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="V16" s="6" t="s">
+      <c r="X16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W16" s="6" t="s">
+      <c r="AC16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X16" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y16" s="6" t="s">
+      <c r="AD16" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE16" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA16" s="9">
-        <v>2000</v>
-      </c>
-      <c r="AB16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD16" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG16" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH16" s="6" t="s">
+      <c r="AF16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG16" s="19">
+        <v>2020</v>
+      </c>
+      <c r="AH16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI16" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ16" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK16" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM16" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI16" s="6" t="s">
+      <c r="AP16" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK16" s="2" t="s">
+      <c r="AQ16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="AS16" t="s">
         <v>106</v>
       </c>
-      <c r="AM16" t="s">
+      <c r="AT16" t="s">
         <v>83</v>
       </c>
-      <c r="AN16" t="s">
-        <v>219</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>220</v>
+      <c r="AU16" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AV16" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>222</v>
+        <v>59</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>224</v>
+        <v>61</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H17" s="12"/>
+      <c r="G17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -3060,178 +3346,239 @@
         <v>64</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>225</v>
+        <v>65</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>66</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W17" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="V17" s="6" t="s">
+      <c r="X17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W17" s="6" t="s">
+      <c r="AC17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X17" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y17" s="6" t="s">
+      <c r="AD17" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE17" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA17" s="9">
+      <c r="AF17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG17" s="9">
         <v>2000</v>
       </c>
-      <c r="AB17" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="AC17" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="AD17" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AE17" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="AF17" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="AG17" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="AH17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN17" s="10"/>
+      <c r="AO17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI17" s="6" t="s">
+      <c r="AP17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ17" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AK17" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>232</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>233</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>234</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>235</v>
+      <c r="AQ17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D18" s="2">
-        <v>9890971</v>
+        <v>222</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>223</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>63</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>156</v>
+      <c r="M18" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>66</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q18" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S18" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="X18" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="Y18" s="6"/>
+      <c r="X18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y18" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="Z18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA18" s="9">
+        <v>227</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG18" s="9">
         <v>2000</v>
       </c>
-      <c r="AH18" s="6"/>
+      <c r="AH18" s="6" t="s">
+        <v>230</v>
+      </c>
       <c r="AI18" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN18" s="10"/>
+      <c r="AO18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK18" s="2" t="s">
-        <v>83</v>
+      <c r="AQ18" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>232</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>233</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>234</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>235</v>
       </c>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>237</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="D19" s="2">
+        <v>9890971</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>62</v>
@@ -3239,216 +3586,299 @@
       <c r="G19" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
       <c r="L19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="O19" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="Z19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI19" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD19" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG19" s="9">
+        <v>2000</v>
+      </c>
+      <c r="AO19" s="6"/>
+      <c r="AP19" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ19" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK19" s="2" t="s">
+      <c r="AQ19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BB19" s="6"/>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>238</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H20" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="AI20" s="6" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP20" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK20" s="2" t="s">
+      <c r="AQ20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR20" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="BI20" s="6"/>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>239</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AP21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ21" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR21" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AJ21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK21" s="2" t="s">
+      <c r="AQ22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AL21" t="s">
+      <c r="AS22" t="s">
         <v>106</v>
       </c>
-      <c r="BB21" s="6" t="s">
+      <c r="BI22" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="BC21" s="2" t="s">
+      <c r="BJ22" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D22" t="s">
-        <v>243</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F22" s="6" t="s">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D23" t="s">
+        <v>273</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="7" t="s">
+      <c r="M23" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="N22" s="6" t="s">
+      <c r="N23" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O22" s="11" t="s">
+      <c r="O23" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="P22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q22" s="8" t="s">
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="W23" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="R22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="S22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T22" s="6" t="s">
+      <c r="X23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z23" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="U22" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="V22" s="6" t="s">
+      <c r="AA23" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="W22" s="6" t="s">
+      <c r="AC23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X22" s="12" t="s">
+      <c r="AD23" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="Y22" s="6" t="s">
+      <c r="AE23" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA22" s="9">
+      <c r="AF23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG23" s="9">
         <v>2000</v>
       </c>
-      <c r="AB22" s="6" t="s">
+      <c r="AH23" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AC22" s="6" t="s">
+      <c r="AI23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AD22" s="6" t="s">
+      <c r="AJ23" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AE22" s="6" t="s">
+      <c r="AK23" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AF22" s="10" t="s">
+      <c r="AL23" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AG22" s="10" t="s">
+      <c r="AM23" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AH22" s="6" t="s">
+      <c r="AN23" s="10"/>
+      <c r="AO23" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AI22" s="6" t="s">
+      <c r="AP23" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AJ22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK22" s="2" t="s">
+      <c r="AQ23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BG22" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="2" t="s">
-        <v>205</v>
+      <c r="BP23" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="5" t="s">
-        <v>206</v>
+      <c r="C41" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="13" t="s">
-        <v>207</v>
+      <c r="C42" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="15" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>